<commit_message>
Fixing UAT Notes 27 Jan 2023
</commit_message>
<xml_diff>
--- a/Web/Content/EMCS/Templates/TemplateCatepillarSparePart.xlsx
+++ b/Web/Content/EMCS/Templates/TemplateCatepillarSparePart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hergy\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9409A4-70DC-41D9-A7D2-706A029378D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77459BE0-43FD-4AD9-9647-9199128DBC42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CIPLItem" sheetId="1" r:id="rId1"/>
@@ -118,9 +118,6 @@
     <t>54.000</t>
   </si>
   <si>
-    <t>23.000</t>
-  </si>
-  <si>
     <t>Uom</t>
   </si>
   <si>
@@ -140,16 +137,25 @@
   </si>
   <si>
     <t>200.00</t>
+  </si>
+  <si>
+    <t>54.001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -461,21 +467,21 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5546875" customWidth="1"/>
-    <col min="5" max="7" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="11" max="19" width="15.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="7" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="11" max="19" width="15.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,7 +492,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -534,9 +540,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>4100184111</v>
+        <v>4100158785</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -545,7 +551,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -554,7 +560,7 @@
         <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H2" t="s">
         <v>21</v>
@@ -590,12 +596,12 @@
         <v>31</v>
       </c>
       <c r="S2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>4100184111</v>
+        <v>4100158785</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -604,7 +610,7 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
@@ -613,10 +619,10 @@
         <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I3" t="s">
         <v>22</v>
@@ -649,12 +655,12 @@
         <v>31</v>
       </c>
       <c r="S3" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>4100184111</v>
+        <v>4100158785</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -663,7 +669,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
@@ -672,10 +678,10 @@
         <v>20</v>
       </c>
       <c r="G4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" t="s">
         <v>37</v>
-      </c>
-      <c r="H4" t="s">
-        <v>38</v>
       </c>
       <c r="I4" t="s">
         <v>22</v>
@@ -708,10 +714,11 @@
         <v>31</v>
       </c>
       <c r="S4" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>